<commit_message>
2018.09.24 - Added Next Song, black BG, and fixed 60 FPS constant
* Next Song is just to change to next song when debugging to make more
interesting (Could randomize too but didn't feel like it...yet)
* blackBG just required me to update PS file, though I just realized I
forgot to see if it was working. Pretty sure it's not. oh well... :P
* 61 > 60 FPS was fixed by this line:
if(timer >= 1000000000) {
it was missing the equals on >=
</commit_message>
<xml_diff>
--- a/res/textures/misc_grid calculations.xlsx
+++ b/res/textures/misc_grid calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apauley\git\luigi-game\luigi-game\res\textures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanp\git\luigi-game\res\textures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DB4F9FAD-708D-421B-8675-E14F4B69A16F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4D5FAE-E211-4F0E-9E57-AD5EAA0BDAF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="11910" xr2:uid="{364E96BE-20B1-4803-B2ED-97527E564539}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>X|Y</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>0569</t>
+  </si>
+  <si>
+    <t>0570</t>
   </si>
 </sst>
 </file>
@@ -741,16 +744,16 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="35" width="9.140625" style="1" customWidth="1"/>
-    <col min="36" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="35" width="9.1796875" style="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
@@ -857,7 +860,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20">
         <v>28</v>
       </c>
@@ -982,7 +985,7 @@
       <c r="AH2" s="17"/>
       <c r="AI2" s="18"/>
     </row>
-    <row r="3" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20">
         <v>33</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>0060</v>
       </c>
     </row>
-    <row r="4" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20">
         <v>28</v>
       </c>
@@ -1247,7 +1250,7 @@
       <c r="AH4" s="11"/>
       <c r="AI4" s="12"/>
     </row>
-    <row r="5" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20">
         <v>33</v>
       </c>
@@ -1387,7 +1390,7 @@
         <v>0121</v>
       </c>
     </row>
-    <row r="6" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20">
         <v>28</v>
       </c>
@@ -1512,7 +1515,7 @@
       <c r="AH6" s="11"/>
       <c r="AI6" s="12"/>
     </row>
-    <row r="7" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20">
         <v>33</v>
       </c>
@@ -1652,7 +1655,7 @@
         <v>0182</v>
       </c>
     </row>
-    <row r="8" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="20">
         <v>28</v>
       </c>
@@ -1777,7 +1780,7 @@
       <c r="AH8" s="11"/>
       <c r="AI8" s="12"/>
     </row>
-    <row r="9" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20">
         <v>33</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>0243</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="20">
         <v>26</v>
       </c>
@@ -2036,7 +2039,7 @@
       <c r="AH10" s="11"/>
       <c r="AI10" s="12"/>
     </row>
-    <row r="11" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="20">
         <v>25</v>
       </c>
@@ -2152,7 +2155,7 @@
       <c r="AH11" s="11"/>
       <c r="AI11" s="12"/>
     </row>
-    <row r="12" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="20">
         <v>26</v>
       </c>
@@ -2271,7 +2274,7 @@
       <c r="AH12" s="11"/>
       <c r="AI12" s="12"/>
     </row>
-    <row r="13" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="20">
         <v>25</v>
       </c>
@@ -2387,7 +2390,7 @@
       <c r="AH13" s="11"/>
       <c r="AI13" s="12"/>
     </row>
-    <row r="14" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20">
         <v>26</v>
       </c>
@@ -2506,7 +2509,7 @@
       <c r="AH14" s="11"/>
       <c r="AI14" s="12"/>
     </row>
-    <row r="15" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="20">
         <v>25</v>
       </c>
@@ -2622,7 +2625,7 @@
       <c r="AH15" s="11"/>
       <c r="AI15" s="12"/>
     </row>
-    <row r="16" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20">
         <v>26</v>
       </c>
@@ -2741,7 +2744,7 @@
       <c r="AH16" s="11"/>
       <c r="AI16" s="12"/>
     </row>
-    <row r="17" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="20">
         <v>25</v>
       </c>
@@ -2857,7 +2860,7 @@
       <c r="AH17" s="11"/>
       <c r="AI17" s="12"/>
     </row>
-    <row r="18" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20">
         <v>26</v>
       </c>
@@ -2976,7 +2979,7 @@
       <c r="AH18" s="11"/>
       <c r="AI18" s="12"/>
     </row>
-    <row r="19" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="20">
         <v>25</v>
       </c>
@@ -3092,7 +3095,7 @@
       <c r="AH19" s="11"/>
       <c r="AI19" s="12"/>
     </row>
-    <row r="20" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20">
         <v>26</v>
       </c>
@@ -3211,7 +3214,7 @@
       <c r="AH20" s="11"/>
       <c r="AI20" s="12"/>
     </row>
-    <row r="21" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20">
         <v>25</v>
       </c>
@@ -3327,7 +3330,7 @@
       <c r="AH21" s="11"/>
       <c r="AI21" s="12"/>
     </row>
-    <row r="22" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20">
         <v>11</v>
       </c>
@@ -3401,7 +3404,7 @@
       <c r="AH22" s="11"/>
       <c r="AI22" s="12"/>
     </row>
-    <row r="23" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20">
         <v>10</v>
       </c>
@@ -3443,8 +3446,8 @@
       <c r="K23" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="L23" s="11">
-        <v>570</v>
+      <c r="L23" s="21" t="s">
+        <v>3</v>
       </c>
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
@@ -3470,7 +3473,7 @@
       <c r="AH23" s="11"/>
       <c r="AI23" s="12"/>
     </row>
-    <row r="24" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20">
         <v>11</v>
       </c>
@@ -3544,7 +3547,7 @@
       <c r="AH24" s="11"/>
       <c r="AI24" s="12"/>
     </row>
-    <row r="25" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="20">
         <v>8</v>
       </c>
@@ -3609,7 +3612,7 @@
       <c r="AH25" s="11"/>
       <c r="AI25" s="12"/>
     </row>
-    <row r="26" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="20">
         <v>11</v>
       </c>
@@ -3683,7 +3686,7 @@
       <c r="AH26" s="11"/>
       <c r="AI26" s="12"/>
     </row>
-    <row r="27" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="20">
         <v>8</v>
       </c>
@@ -3748,7 +3751,7 @@
       <c r="AH27" s="11"/>
       <c r="AI27" s="12"/>
     </row>
-    <row r="28" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="20">
         <v>11</v>
       </c>
@@ -3822,7 +3825,7 @@
       <c r="AH28" s="11"/>
       <c r="AI28" s="12"/>
     </row>
-    <row r="29" spans="1:35" s="2" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" s="2" customFormat="1" ht="50.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="20">
         <v>8</v>
       </c>
@@ -3899,7 +3902,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3911,7 +3914,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3923,7 +3926,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>